<commit_message>
Added columns for first name, last name and sub address
</commit_message>
<xml_diff>
--- a/Day_19_Custom_YOLO/output.xlsx
+++ b/Day_19_Custom_YOLO/output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E77"/>
+  <dimension ref="A1:H67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,17 +434,40 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="B1" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="n">
-        <v>3</v>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Names of Electors in full, Surname being first</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Place of Abode</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Nature of Qualification</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Description of Qualifying Property</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>First Name</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Last Name</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Sub Address</t>
+        </is>
       </c>
     </row>
     <row r="2">
@@ -453,14 +476,37 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Names of Electors in full , Surname</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr"/>
+          <t>Evans , Thomas</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>11 , Park lane</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>dwelling house</t>
+        </is>
+      </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Description of Qualifying</t>
+          <t>11 Park lane</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Evans </t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Thomas</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>PARK LANE</t>
         </is>
       </c>
     </row>
@@ -470,22 +516,37 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>being first</t>
+          <t>Francis , Thomas</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Place of Abode</t>
+          <t>2 , Park lane</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Nature of Qualification</t>
+          <t>dwelling house</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Property</t>
+          <t>2 , Park lane</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Francis </t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Thomas</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>PARK LANE</t>
         </is>
       </c>
     </row>
@@ -493,18 +554,41 @@
       <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B4" t="inlineStr"/>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Griffiths , William</t>
+        </is>
+      </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>PARK</t>
+          <t>9 , Park lane</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>LANE</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr"/>
+          <t>dwelling house</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>9 , Park lane</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Griffiths </t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> William</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>PARK LANE</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -512,12 +596,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Evans , Thomas</t>
+          <t>Howells , John</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>11 , Park lane</t>
+          <t>7 , Park lane</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -527,7 +611,22 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>11 Park lane</t>
+          <t>7 , Park lane</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Howells </t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> John</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>PARK LANE</t>
         </is>
       </c>
     </row>
@@ -537,12 +636,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Francis , Thomas</t>
+          <t>Jones , William</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>2 , Park lane</t>
+          <t>5 , Park lane</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -552,7 +651,22 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2 , Park lane</t>
+          <t>5 , Park lane</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Jones </t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> William</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>PARK LANE</t>
         </is>
       </c>
     </row>
@@ -562,12 +676,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Griffiths , William</t>
+          <t>Jones , David</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>9 , Park lane</t>
+          <t>o , Park lane</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -577,7 +691,22 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>9 , Park lane</t>
+          <t>6 , Park lane</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Jones </t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> David</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>PARK LANE</t>
         </is>
       </c>
     </row>
@@ -587,12 +716,12 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Howells , John</t>
+          <t>Wilson , William</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>7 , Park lane</t>
+          <t>3 , Park lane</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -602,7 +731,22 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>7 , Park lane</t>
+          <t>3 , Park lane</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Wilson </t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> William</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>PARK LANE</t>
         </is>
       </c>
     </row>
@@ -612,12 +756,12 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Jones , William</t>
+          <t>Williams , David</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>5 , Park lane</t>
+          <t>8 , Park lare</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -627,7 +771,22 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>5 , Park lane</t>
+          <t>18 , Park lane</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Williams </t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> David</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>PARK LANE</t>
         </is>
       </c>
     </row>
@@ -637,12 +796,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Jones , David</t>
+          <t>Bentley , Frank</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>o , Park lane</t>
+          <t>Murray street</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -652,7 +811,22 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>6 , Park lane</t>
+          <t>Murray street</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Bentley </t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Frank</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>MURRAY STREET</t>
         </is>
       </c>
     </row>
@@ -662,12 +836,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Wilson , William</t>
+          <t>Coombs , Frederick</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>3 , Park lane</t>
+          <t>Murray street</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -677,7 +851,22 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>3 , Park lane</t>
+          <t>Murray street</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Coombs </t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Frederick</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>MURRAY STREET</t>
         </is>
       </c>
     </row>
@@ -687,22 +876,37 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Williams , David</t>
+          <t>Davies , David James</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>8 , Park lare</t>
+          <t>Murray street</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>dwelling house</t>
+          <t>tenement , joint</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>18 , Park lane</t>
+          <t>Murray street</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Davies </t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> David James</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>MURRAY STREET</t>
         </is>
       </c>
     </row>
@@ -710,18 +914,41 @@
       <c r="A13" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="B13" t="inlineStr"/>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Davies , William</t>
+        </is>
+      </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>MURRAY</t>
+          <t>Murray street</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>STREET</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr"/>
+          <t>dwelling house</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Murray street</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Davies </t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> William</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>MURRAY STREET</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
@@ -729,12 +956,12 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Bentley , Frank</t>
+          <t>Hopkins , William</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Murray street</t>
+          <t>Murray street ( Raven Inn )</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -745,6 +972,21 @@
       <c r="E14" t="inlineStr">
         <is>
           <t>Murray street</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hopkins </t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> William</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>MURRAY STREET</t>
         </is>
       </c>
     </row>
@@ -754,7 +996,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Coombs , Frederick</t>
+          <t>Henry , Gavin</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -770,6 +1012,21 @@
       <c r="E15" t="inlineStr">
         <is>
           <t>Murray street</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Henry </t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Gavin</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>MURRAY STREET</t>
         </is>
       </c>
     </row>
@@ -779,7 +1036,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Davies , David James</t>
+          <t>Jones , William</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -789,12 +1046,27 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>tenement , joint</t>
+          <t>dwelling house</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
           <t>Murray street</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Jones </t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> William</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>MURRAY STREET</t>
         </is>
       </c>
     </row>
@@ -804,7 +1076,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Davies , William</t>
+          <t>Jones , William B</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -814,12 +1086,27 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>dwelling house</t>
+          <t>tenement</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
           <t>Murray street</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Jones </t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> William B</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>MURRAY STREET</t>
         </is>
       </c>
     </row>
@@ -829,12 +1116,12 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Hopkins , William</t>
+          <t>Jones , Evan</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Murray street ( Raven Inn )</t>
+          <t>Murray street ( Bres Cottage )</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -845,6 +1132,21 @@
       <c r="E18" t="inlineStr">
         <is>
           <t>Murray street</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Jones </t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Evan</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>MURRAY STREET</t>
         </is>
       </c>
     </row>
@@ -854,7 +1156,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Henry , Gavin</t>
+          <t>Lloyd , John Jenkin</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -870,6 +1172,21 @@
       <c r="E19" t="inlineStr">
         <is>
           <t>Murray street</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Lloyd </t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> John Jenkin</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>MURRAY STREET</t>
         </is>
       </c>
     </row>
@@ -879,12 +1196,12 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Jones , William</t>
+          <t>Mackie , William</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Murray street</t>
+          <t>Murray street ( Clarence Hotel )</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -895,6 +1212,21 @@
       <c r="E20" t="inlineStr">
         <is>
           <t>Murray street</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mackie </t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> William</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>MURRAY STREET</t>
         </is>
       </c>
     </row>
@@ -904,7 +1236,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Jones , William B</t>
+          <t>Newmark , Louis</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -914,12 +1246,27 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>tenement</t>
+          <t>dwelling house</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
           <t>Murray street</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Newmark </t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Louis</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>MURRAY STREET</t>
         </is>
       </c>
     </row>
@@ -929,12 +1276,12 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Jones , Evan</t>
+          <t>Rowe , William</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Murray street ( Bres Cottage )</t>
+          <t>Murray street</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -945,6 +1292,21 @@
       <c r="E22" t="inlineStr">
         <is>
           <t>Murray street</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Rowe </t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> William</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>MURRAY STREET</t>
         </is>
       </c>
     </row>
@@ -954,7 +1316,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Lloyd , John Jenkin</t>
+          <t>Reubenstein , Morris</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -970,6 +1332,21 @@
       <c r="E23" t="inlineStr">
         <is>
           <t>Murray street</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Reubenstein </t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Morris</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>MURRAY STREET</t>
         </is>
       </c>
     </row>
@@ -979,12 +1356,12 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Mackie , William</t>
+          <t>Reubenstein , Harris</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Murray street ( Clarence Hotel )</t>
+          <t>Murray street</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -995,6 +1372,21 @@
       <c r="E24" t="inlineStr">
         <is>
           <t>Murray street</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Reubenstein </t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Harris</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>MURRAY STREET</t>
         </is>
       </c>
     </row>
@@ -1004,7 +1396,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Newmark , Louis</t>
+          <t>Stevenson , George</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1020,6 +1412,21 @@
       <c r="E25" t="inlineStr">
         <is>
           <t>Murray street</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Stevenson </t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> George</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>MURRAY STREET</t>
         </is>
       </c>
     </row>
@@ -1029,22 +1436,37 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Rowe , William</t>
+          <t>Thomas , James</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Murray street</t>
+          <t>Muraay street</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>dwelling house</t>
+          <t>dwelling house and shop</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
           <t>Murray street</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Thomas </t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> James</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>MURRAY STREET</t>
         </is>
       </c>
     </row>
@@ -1054,7 +1476,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Reubenstein , Morris</t>
+          <t>Thomas , Evan , junior</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1064,12 +1486,27 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>dwelling house</t>
+          <t>dwelling house and shop</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
           <t>Murray street</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Thomas </t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Evan </t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>MURRAY STREET</t>
         </is>
       </c>
     </row>
@@ -1079,12 +1516,12 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Reubenstein , Harris</t>
+          <t>Thomas , W G</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Murray street</t>
+          <t>Murray street ( Malabar )</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -1095,6 +1532,21 @@
       <c r="E28" t="inlineStr">
         <is>
           <t>Murray street</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Thomas </t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> W G</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>MURRAY STREET</t>
         </is>
       </c>
     </row>
@@ -1104,7 +1556,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Stevenson , George</t>
+          <t>Thomas , Jonah</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1120,6 +1572,21 @@
       <c r="E29" t="inlineStr">
         <is>
           <t>Murray street</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Thomas </t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Jonah</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>MURRAY STREET</t>
         </is>
       </c>
     </row>
@@ -1129,22 +1596,37 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Thomas , James</t>
+          <t>Thomas , Thomas</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Muraay street</t>
+          <t>Murray street ( Albion Inn )</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>dwelling house and shop</t>
+          <t>dwelling house</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
           <t>Murray street</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Thomas </t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Thomas</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>MURRAY STREET</t>
         </is>
       </c>
     </row>
@@ -1154,7 +1636,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Thomas , Evan , junior</t>
+          <t>Vivian , Frank</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1164,12 +1646,27 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>dwelling house and shop</t>
+          <t>dwelling house</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
           <t>Murray street</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Vivian </t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Frank</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>MURRAY STREET</t>
         </is>
       </c>
     </row>
@@ -1179,12 +1676,12 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Thomas , W G</t>
+          <t>Williams , Willia</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Murray street ( Malabar )</t>
+          <t>Murray street</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -1195,6 +1692,21 @@
       <c r="E32" t="inlineStr">
         <is>
           <t>Murray street</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Williams </t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Willia</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>MURRAY STREET</t>
         </is>
       </c>
     </row>
@@ -1204,12 +1716,12 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Thomas , Jonah</t>
+          <t>Williams , John</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Murray street</t>
+          <t>Murray st ( Pretoria house )</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -1220,6 +1732,21 @@
       <c r="E33" t="inlineStr">
         <is>
           <t>Murray street</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Williams </t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> John</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>MURRAY STREET</t>
         </is>
       </c>
     </row>
@@ -1229,12 +1756,12 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Thomas , Thomas</t>
+          <t>Davey , W A</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Murray street ( Albion Inn )</t>
+          <t>1 , Greenfield Villas</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -1244,7 +1771,22 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>Murray street</t>
+          <t>I , Greenfield Villas</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Davey </t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> W A</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>GREENFIELD VILLAS</t>
         </is>
       </c>
     </row>
@@ -1254,12 +1796,12 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Vivian , Frank</t>
+          <t>Arnold , Thomas</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Murray street</t>
+          <t>Loughor</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -1269,7 +1811,22 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>Murray street</t>
+          <t>Greenfield Villas</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Arnold </t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Thomas</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>GREENFIELD VILLAS</t>
         </is>
       </c>
     </row>
@@ -1279,12 +1836,12 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Williams , Willia</t>
+          <t>Evans , William O</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Murray street</t>
+          <t>5 , Greenfield Villas</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -1294,7 +1851,22 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>Murray street</t>
+          <t>5 , Greenfield Villas</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Evans </t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> William O</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>GREENFIELD VILLAS</t>
         </is>
       </c>
     </row>
@@ -1304,22 +1876,37 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Williams , John</t>
+          <t>Edmunds , Robert J</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Murray st ( Pretoria house )</t>
+          <t>11 II , , Greenfield Villas</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>dwelling house</t>
+          <t>dwelling house ………</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>Murray street</t>
+          <t>11 , Greenfield Villas</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Edmunds </t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Robert J</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>GREENFIELD VILLAS</t>
         </is>
       </c>
     </row>
@@ -1327,18 +1914,41 @@
       <c r="A38" s="1" t="n">
         <v>36</v>
       </c>
-      <c r="B38" t="inlineStr"/>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Jones , W E</t>
+        </is>
+      </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>GREENFIELD</t>
+          <t>3 , Greenfield Villas</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>VILLAS</t>
-        </is>
-      </c>
-      <c r="E38" t="inlineStr"/>
+          <t>dwelling house</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>3 , Greenfield Villas</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Jones </t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> W E</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>GREENFIELD VILLAS</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
@@ -1346,12 +1956,12 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Davey , W A</t>
+          <t>Lewis , Thomas D</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>1 , Greenfield Villas</t>
+          <t>7 , Greenfield Villas</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -1361,7 +1971,22 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>I , Greenfield Villas</t>
+          <t>7 , Greenfield Villas</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Lewis </t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Thomas D</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>GREENFIELD VILLAS</t>
         </is>
       </c>
     </row>
@@ -1371,12 +1996,12 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Arnold , Thomas</t>
+          <t>Phillips , Douglas</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Loughor</t>
+          <t>Greenfield Villas</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -1387,6 +2012,21 @@
       <c r="E40" t="inlineStr">
         <is>
           <t>Greenfield Villas</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phillips </t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Douglas</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>GREENFIELD VILLAS</t>
         </is>
       </c>
     </row>
@@ -1396,12 +2036,12 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Evans , William O</t>
+          <t>Owen , Luther</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>5 , Greenfield Villas</t>
+          <t>21 , Greenfield Villas</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -1411,7 +2051,22 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>5 , Greenfield Villas</t>
+          <t>21 , Greenfield Villas</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Owen </t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Luther</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>GREENFIELD VILLAS</t>
         </is>
       </c>
     </row>
@@ -1421,22 +2076,37 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Edmunds , Robert J</t>
+          <t>Shrivelle , Alfred G</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>11 II , , Greenfield Villas</t>
+          <t>23 , Greenfield Villas</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>dwelling house ………</t>
+          <t>dwelling house</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>11 , Greenfield Villas</t>
+          <t>23 , Greenfield Villas</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Shrivelle </t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Alfred G</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>GREENFIELD VILLAS</t>
         </is>
       </c>
     </row>
@@ -1446,12 +2116,12 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Jones , W E</t>
+          <t>Thomas , Evan</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>3 , Greenfield Villas</t>
+          <t>19 , Greenfield Villas</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -1461,7 +2131,22 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>3 , Greenfield Villas</t>
+          <t>19 , Greenfield Villas</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Thomas </t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Evan</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>GREENFIELD VILLAS</t>
         </is>
       </c>
     </row>
@@ -1471,22 +2156,37 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Lewis , Thomas D</t>
+          <t>Beynon , W P</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>7 , Greenfield Villas</t>
+          <t>2 , Greenfield terrace</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>dwelling house</t>
+          <t>dwelling house , successive</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>7 , Greenfield Villas</t>
+          <t>2 , Greenfield terrace and IT</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Beynon </t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> W P</t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>GREENFIELD TERRACE</t>
         </is>
       </c>
     </row>
@@ -1496,12 +2196,12 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Phillips , Douglas</t>
+          <t>Clement , John</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Greenfield Villas</t>
+          <t>16 , Greenfield terrace</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -1511,7 +2211,22 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>Greenfield Villas</t>
+          <t>16 , Greenfield terrace</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Clement </t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> John</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>John street</t>
         </is>
       </c>
     </row>
@@ -1521,12 +2236,12 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Owen , Luther</t>
+          <t>Davies , Thomas Dixon</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>21 , Greenfield Villas</t>
+          <t>8 , Greenfield terrace</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -1536,7 +2251,22 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>21 , Greenfield Villas</t>
+          <t>8 , Greenfield terrace</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Davies </t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Thomas Dixon</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>John street</t>
         </is>
       </c>
     </row>
@@ -1546,12 +2276,12 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Shrivelle , Alfred G</t>
+          <t>Evans , David John</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>23 , Greenfield Villas</t>
+          <t>10 , Greenfield terrace</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -1561,7 +2291,22 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>23 , Greenfield Villas</t>
+          <t>10 , Greenfield terrace</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Evans </t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> David John</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>John street</t>
         </is>
       </c>
     </row>
@@ -1571,12 +2316,12 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Thomas , Evan</t>
+          <t>Hopkins , Griffiths</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>19 , Greenfield Villas</t>
+          <t>12 , Greenfield terrace</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -1586,7 +2331,22 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>19 , Greenfield Villas</t>
+          <t>12 , Greenfield terrace</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hopkins </t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Griffiths</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>John street</t>
         </is>
       </c>
     </row>
@@ -1594,18 +2354,41 @@
       <c r="A49" s="1" t="n">
         <v>47</v>
       </c>
-      <c r="B49" t="inlineStr"/>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Johns , Rev Thomas</t>
+        </is>
+      </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>GREENFIELD</t>
+          <t>18 , Greenfield terrace</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>TERRACE</t>
-        </is>
-      </c>
-      <c r="E49" t="inlineStr"/>
+          <t>dwelling house ……</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>18 , Greenfield terrace</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Johns </t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Rev Thomas</t>
+        </is>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>John street</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
@@ -1613,22 +2396,37 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Beynon , W P</t>
+          <t>Linn , Robert H</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>2 , Greenfield terrace</t>
+          <t>22 , Greenfield terrace</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>dwelling house , successive</t>
+          <t>dwelling house</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>2 , Greenfield terrace and IT</t>
+          <t>22 , Greenfield terrace</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Linn </t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Robert H</t>
+        </is>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>John street</t>
         </is>
       </c>
     </row>
@@ -1636,10 +2434,37 @@
       <c r="A51" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="B51" t="inlineStr"/>
-      <c r="C51" t="inlineStr"/>
-      <c r="D51" t="inlineStr"/>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Rees , Frederick</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>4 , Greenfield terrace</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>dwelling house</t>
+        </is>
+      </c>
       <c r="E51" t="inlineStr">
+        <is>
+          <t>4 , Greenfield terrace</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Rees </t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Frederick</t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr">
         <is>
           <t>John street</t>
         </is>
@@ -1651,12 +2476,12 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Clement , John</t>
+          <t>Williams , John Owen</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>16 , Greenfield terrace</t>
+          <t>6 , Greenfield terrace</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
@@ -1666,7 +2491,22 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>16 , Greenfield terrace</t>
+          <t>6 , Greenfield terrace</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Williams </t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> John Owen</t>
+        </is>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>John street</t>
         </is>
       </c>
     </row>
@@ -1676,12 +2516,12 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Davies , Thomas Dixon</t>
+          <t>Brown , James</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>8 , Greenfield terrace</t>
+          <t>13 , Upper Inkerman street</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
@@ -1691,7 +2531,22 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>8 , Greenfield terrace</t>
+          <t>13 , Upper Inkerman street</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Brown </t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> James</t>
+        </is>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>UPPER INKERMAN STREET</t>
         </is>
       </c>
     </row>
@@ -1701,12 +2556,12 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Evans , David John</t>
+          <t>Davies , Evan</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>10 , Greenfield terrace</t>
+          <t>1 , Upper Inkerman street</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
@@ -1716,7 +2571,22 @@
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>10 , Greenfield terrace</t>
+          <t>1 , Upper Inkerman street</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Davies </t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Evan</t>
+        </is>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>UPPER INKERMAN STREET</t>
         </is>
       </c>
     </row>
@@ -1726,12 +2596,12 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Hopkins , Griffiths</t>
+          <t>Jacob , J H</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>12 , Greenfield terrace</t>
+          <t>2 , Upper Inkerman street</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
@@ -1741,7 +2611,22 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>12 , Greenfield terrace</t>
+          <t>2 , Upper Inkelman street</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Jacob </t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> J H</t>
+        </is>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>UPPER INKERMAN STREET</t>
         </is>
       </c>
     </row>
@@ -1751,22 +2636,37 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Johns , Rev Thomas</t>
+          <t>Lewis , Samuel</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>18 , Greenfield terrace</t>
+          <t>6 , Upper Inkerman street</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>dwelling house ……</t>
+          <t>dwelling house</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>18 , Greenfield terrace</t>
+          <t>6 , Upper Inkerman street</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Lewis </t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Samuel</t>
+        </is>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>UPPER INKERMAN STREET</t>
         </is>
       </c>
     </row>
@@ -1776,12 +2676,12 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Linn , Robert H</t>
+          <t>Lovett , Joseph |</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>22 , Greenfield terrace</t>
+          <t>4 , Upper Inkerman street</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
@@ -1791,7 +2691,22 @@
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>22 , Greenfield terrace</t>
+          <t>4 , Upper Inkerman street</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Lovett </t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Joseph |</t>
+        </is>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>UPPER INKERMAN STREET</t>
         </is>
       </c>
     </row>
@@ -1801,12 +2716,12 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Rees , Frederick</t>
+          <t>Price , William Henry</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>4 , Greenfield terrace</t>
+          <t>10a , Upper Inkerman street</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
@@ -1816,7 +2731,22 @@
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>4 , Greenfield terrace</t>
+          <t>10a , Upper Inkerman street</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Price </t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> William Henry</t>
+        </is>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>UPPER INKERMAN STREET</t>
         </is>
       </c>
     </row>
@@ -1826,12 +2756,12 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Williams , John Owen</t>
+          <t>Thomas , Walter</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>6 , Greenfield terrace</t>
+          <t>5 , Upper Inkerman street</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
@@ -1841,7 +2771,22 @@
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>6 , Greenfield terrace</t>
+          <t>5 , Upper Inkerman street</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Thomas </t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Walter</t>
+        </is>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>UPPER INKERMAN STREET</t>
         </is>
       </c>
     </row>
@@ -1849,18 +2794,41 @@
       <c r="A60" s="1" t="n">
         <v>58</v>
       </c>
-      <c r="B60" t="inlineStr"/>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>Thomas , William</t>
+        </is>
+      </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>UPPER</t>
+          <t>7 , Upper Inkerman street</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>INKERMAN STREET</t>
-        </is>
-      </c>
-      <c r="E60" t="inlineStr"/>
+          <t>dwelling house</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>7 , Upper Inkerman street</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Thomas </t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> William</t>
+        </is>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>UPPER INKERMAN STREET</t>
+        </is>
+      </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
@@ -1868,12 +2836,12 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Brown , James</t>
+          <t>Williams , John</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>13 , Upper Inkerman street</t>
+          <t>9a , Upper Inkerman street</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
@@ -1883,7 +2851,22 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>13 , Upper Inkerman street</t>
+          <t>ya , Upper Inkerman street</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Williams </t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> John</t>
+        </is>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>UPPER INKERMAN STREET</t>
         </is>
       </c>
     </row>
@@ -1893,12 +2876,12 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Davies , Evan</t>
+          <t>Williams , Daniel</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>1 , Upper Inkerman street</t>
+          <t>8 , Upper Inkerman street</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
@@ -1908,7 +2891,22 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>1 , Upper Inkerman street</t>
+          <t>8 , Upper Inkerman street</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Williams </t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Daniel</t>
+        </is>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>UPPER INKERMAN STREET</t>
         </is>
       </c>
     </row>
@@ -1918,12 +2916,12 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Jacob , J H</t>
+          <t>Williams , John</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>2 , Upper Inkerman street</t>
+          <t>9 , Upper Inkerman street</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
@@ -1933,7 +2931,22 @@
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>2 , Upper Inkelman street</t>
+          <t>9 , Upper Inkerman street</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Williams </t>
+        </is>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> John</t>
+        </is>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>UPPER INKERMAN STREET</t>
         </is>
       </c>
     </row>
@@ -1943,12 +2956,12 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Lewis , Samuel</t>
+          <t>Williams , Daniel</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>6 , Upper Inkerman street</t>
+          <t>10 , Upper Inkerman street</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
@@ -1958,7 +2971,22 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>6 , Upper Inkerman street</t>
+          <t>10 , Upper Inkerman street</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Williams </t>
+        </is>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Daniel</t>
+        </is>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>UPPER INKERMAN STREET</t>
         </is>
       </c>
     </row>
@@ -1968,12 +2996,12 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Lovett , Joseph |</t>
+          <t>Arthur , Luther</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>4 , Upper Inkerman street</t>
+          <t>22 , Inkerman street</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
@@ -1983,7 +3011,22 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>4 , Upper Inkerman street</t>
+          <t>, Inkerman street</t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Arthur </t>
+        </is>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Luther</t>
+        </is>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>INKERMAN STREET</t>
         </is>
       </c>
     </row>
@@ -1993,12 +3036,12 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Price , William Henry</t>
+          <t>Davies , David</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>10a , Upper Inkerman street</t>
+          <t>27 , Inkerman street</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
@@ -2008,7 +3051,22 @@
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>10a , Upper Inkerman street</t>
+          <t>27 , Inkerman street</t>
+        </is>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Davies </t>
+        </is>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> David</t>
+        </is>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>INKERMAN STREET</t>
         </is>
       </c>
     </row>
@@ -2018,248 +3076,37 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Thomas , Walter</t>
+          <t>Davies , John</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>5 , Upper Inkerman street</t>
+          <t>18 , Inkerman street</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>dwelling house</t>
+          <t>dwelling house …</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>5 , Upper Inkerman street</t>
-        </is>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" s="1" t="n">
-        <v>66</v>
-      </c>
-      <c r="B68" t="inlineStr">
-        <is>
-          <t>Thomas , William</t>
-        </is>
-      </c>
-      <c r="C68" t="inlineStr">
-        <is>
-          <t>7 , Upper Inkerman street</t>
-        </is>
-      </c>
-      <c r="D68" t="inlineStr">
-        <is>
-          <t>dwelling house</t>
-        </is>
-      </c>
-      <c r="E68" t="inlineStr">
-        <is>
-          <t>7 , Upper Inkerman street</t>
-        </is>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" s="1" t="n">
-        <v>67</v>
-      </c>
-      <c r="B69" t="inlineStr">
-        <is>
-          <t>Williams , John</t>
-        </is>
-      </c>
-      <c r="C69" t="inlineStr">
-        <is>
-          <t>9a , Upper Inkerman street</t>
-        </is>
-      </c>
-      <c r="D69" t="inlineStr">
-        <is>
-          <t>dwelling house</t>
-        </is>
-      </c>
-      <c r="E69" t="inlineStr">
-        <is>
-          <t>ya , Upper Inkerman street</t>
-        </is>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" s="1" t="n">
-        <v>68</v>
-      </c>
-      <c r="B70" t="inlineStr">
-        <is>
-          <t>Williams , Daniel</t>
-        </is>
-      </c>
-      <c r="C70" t="inlineStr">
-        <is>
-          <t>8 , Upper Inkerman street</t>
-        </is>
-      </c>
-      <c r="D70" t="inlineStr">
-        <is>
-          <t>dwelling house</t>
-        </is>
-      </c>
-      <c r="E70" t="inlineStr">
-        <is>
-          <t>8 , Upper Inkerman street</t>
-        </is>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" s="1" t="n">
-        <v>69</v>
-      </c>
-      <c r="B71" t="inlineStr">
-        <is>
-          <t>Williams , John</t>
-        </is>
-      </c>
-      <c r="C71" t="inlineStr">
-        <is>
-          <t>9 , Upper Inkerman street</t>
-        </is>
-      </c>
-      <c r="D71" t="inlineStr">
-        <is>
-          <t>dwelling house</t>
-        </is>
-      </c>
-      <c r="E71" t="inlineStr">
-        <is>
-          <t>9 , Upper Inkerman street</t>
-        </is>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" s="1" t="n">
-        <v>70</v>
-      </c>
-      <c r="B72" t="inlineStr">
-        <is>
-          <t>Williams , Daniel</t>
-        </is>
-      </c>
-      <c r="C72" t="inlineStr">
-        <is>
-          <t>10 , Upper Inkerman street</t>
-        </is>
-      </c>
-      <c r="D72" t="inlineStr">
-        <is>
-          <t>dwelling house</t>
-        </is>
-      </c>
-      <c r="E72" t="inlineStr">
-        <is>
-          <t>10 , Upper Inkerman street</t>
-        </is>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" s="1" t="n">
-        <v>71</v>
-      </c>
-      <c r="B73" t="inlineStr"/>
-      <c r="C73" t="inlineStr"/>
-      <c r="D73" t="inlineStr"/>
-      <c r="E73" t="inlineStr"/>
-    </row>
-    <row r="74">
-      <c r="A74" s="1" t="n">
-        <v>72</v>
-      </c>
-      <c r="B74" t="inlineStr"/>
-      <c r="C74" t="inlineStr">
-        <is>
-          <t>INKERMAN</t>
-        </is>
-      </c>
-      <c r="D74" t="inlineStr">
-        <is>
-          <t>STREET</t>
-        </is>
-      </c>
-      <c r="E74" t="inlineStr"/>
-    </row>
-    <row r="75">
-      <c r="A75" s="1" t="n">
-        <v>73</v>
-      </c>
-      <c r="B75" t="inlineStr">
-        <is>
-          <t>Arthur , Luther</t>
-        </is>
-      </c>
-      <c r="C75" t="inlineStr">
-        <is>
-          <t>22 , Inkerman street</t>
-        </is>
-      </c>
-      <c r="D75" t="inlineStr">
-        <is>
-          <t>dwelling house</t>
-        </is>
-      </c>
-      <c r="E75" t="inlineStr">
-        <is>
-          <t>, Inkerman street</t>
-        </is>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" s="1" t="n">
-        <v>74</v>
-      </c>
-      <c r="B76" t="inlineStr">
-        <is>
-          <t>Davies , David</t>
-        </is>
-      </c>
-      <c r="C76" t="inlineStr">
-        <is>
-          <t>27 , Inkerman street</t>
-        </is>
-      </c>
-      <c r="D76" t="inlineStr">
-        <is>
-          <t>dwelling house</t>
-        </is>
-      </c>
-      <c r="E76" t="inlineStr">
-        <is>
-          <t>27 , Inkerman street</t>
-        </is>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" s="1" t="n">
-        <v>75</v>
-      </c>
-      <c r="B77" t="inlineStr">
-        <is>
-          <t>Davies , John</t>
-        </is>
-      </c>
-      <c r="C77" t="inlineStr">
-        <is>
           <t>18 , Inkerman street</t>
         </is>
       </c>
-      <c r="D77" t="inlineStr">
-        <is>
-          <t>dwelling house …</t>
-        </is>
-      </c>
-      <c r="E77" t="inlineStr">
-        <is>
-          <t>18 , Inkerman street</t>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Davies </t>
+        </is>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> John</t>
+        </is>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>INKERMAN STREET</t>
         </is>
       </c>
     </row>

</xml_diff>